<commit_message>
/ ‘Extended Campuses/Self Appraisals/2015/Raw Data from SQL Query for 2015.xlsx’
</commit_message>
<xml_diff>
--- a/Extended Campuses/Self Appraisals/2015/Raw Data from SQL Query for 2015.xlsx
+++ b/Extended Campuses/Self Appraisals/2015/Raw Data from SQL Query for 2015.xlsx
@@ -1787,8 +1787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J438"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="G94" sqref="G94"/>
+    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
+      <selection activeCell="H174" sqref="H174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3914,6 +3914,12 @@
       <c r="F98" s="1">
         <v>1</v>
       </c>
+      <c r="H98" s="1">
+        <v>1</v>
+      </c>
+      <c r="I98" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="99" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
@@ -3934,6 +3940,12 @@
       <c r="F99" s="1">
         <v>1</v>
       </c>
+      <c r="H99" s="1">
+        <v>1</v>
+      </c>
+      <c r="I99" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="100" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
@@ -3954,6 +3966,9 @@
       <c r="F100" s="1">
         <v>1</v>
       </c>
+      <c r="I100" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="101" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
@@ -3972,6 +3987,9 @@
         <v>123</v>
       </c>
       <c r="F101" s="1">
+        <v>1</v>
+      </c>
+      <c r="H101" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4093,7 +4111,9 @@
       <c r="H106" s="4">
         <v>1</v>
       </c>
-      <c r="I106" s="4"/>
+      <c r="I106" s="4">
+        <v>1</v>
+      </c>
       <c r="J106" s="4">
         <v>1</v>
       </c>
@@ -4121,7 +4141,9 @@
       <c r="H107" s="4">
         <v>1</v>
       </c>
-      <c r="I107" s="4"/>
+      <c r="I107" s="4">
+        <v>1</v>
+      </c>
       <c r="J107" s="4"/>
     </row>
     <row r="108" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -4225,6 +4247,9 @@
       <c r="E112" s="3" t="s">
         <v>136</v>
       </c>
+      <c r="I112" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="113" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
@@ -4362,7 +4387,9 @@
       <c r="G119" s="4">
         <v>1</v>
       </c>
-      <c r="H119" s="4"/>
+      <c r="H119" s="4">
+        <v>1</v>
+      </c>
       <c r="I119" s="4"/>
       <c r="J119" s="4"/>
     </row>
@@ -4528,6 +4555,9 @@
       <c r="G126" s="1">
         <v>1</v>
       </c>
+      <c r="I126" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="127" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
@@ -4551,6 +4581,9 @@
       <c r="G127" s="1">
         <v>1</v>
       </c>
+      <c r="H127" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="128" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
@@ -4622,7 +4655,9 @@
       <c r="F131" s="4"/>
       <c r="G131" s="4"/>
       <c r="H131" s="4"/>
-      <c r="I131" s="4"/>
+      <c r="I131" s="4">
+        <v>1</v>
+      </c>
       <c r="J131" s="4"/>
     </row>
     <row r="132" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -4648,7 +4683,9 @@
         <v>1</v>
       </c>
       <c r="H132" s="4"/>
-      <c r="I132" s="4"/>
+      <c r="I132" s="4">
+        <v>1</v>
+      </c>
       <c r="J132" s="4"/>
     </row>
     <row r="133" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -4975,7 +5012,9 @@
       </c>
       <c r="G146" s="4"/>
       <c r="H146" s="4"/>
-      <c r="I146" s="4"/>
+      <c r="I146" s="4">
+        <v>1</v>
+      </c>
       <c r="J146" s="4">
         <v>1</v>
       </c>
@@ -5027,7 +5066,9 @@
       </c>
       <c r="G148" s="4"/>
       <c r="H148" s="4"/>
-      <c r="I148" s="4"/>
+      <c r="I148" s="4">
+        <v>1</v>
+      </c>
       <c r="J148" s="4"/>
     </row>
     <row r="149" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -5053,7 +5094,9 @@
         <v>1</v>
       </c>
       <c r="H149" s="4"/>
-      <c r="I149" s="4"/>
+      <c r="I149" s="4">
+        <v>1</v>
+      </c>
       <c r="J149" s="4"/>
     </row>
     <row r="150" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -5077,7 +5120,9 @@
       </c>
       <c r="G150" s="4"/>
       <c r="H150" s="4"/>
-      <c r="I150" s="4"/>
+      <c r="I150" s="4">
+        <v>1</v>
+      </c>
       <c r="J150" s="4"/>
     </row>
     <row r="151" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -5121,6 +5166,12 @@
       <c r="F152" s="1">
         <v>1</v>
       </c>
+      <c r="H152" s="1">
+        <v>1</v>
+      </c>
+      <c r="I152" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="153" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
@@ -5164,6 +5215,9 @@
       <c r="F154" s="1">
         <v>1</v>
       </c>
+      <c r="I154" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="155" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
@@ -5184,6 +5238,9 @@
       <c r="F155" s="1">
         <v>1</v>
       </c>
+      <c r="H155" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="156" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
@@ -5204,6 +5261,12 @@
       <c r="F156" s="1">
         <v>1</v>
       </c>
+      <c r="H156" s="1">
+        <v>1</v>
+      </c>
+      <c r="I156" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="157" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
@@ -5227,6 +5290,9 @@
       <c r="G157" s="1">
         <v>1</v>
       </c>
+      <c r="H157" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="158" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
@@ -5250,6 +5316,9 @@
       <c r="G158" s="1">
         <v>1</v>
       </c>
+      <c r="H158" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="159" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
@@ -5307,8 +5376,12 @@
       <c r="G161" s="4">
         <v>1</v>
       </c>
-      <c r="H161" s="4"/>
-      <c r="I161" s="4"/>
+      <c r="H161" s="4">
+        <v>1</v>
+      </c>
+      <c r="I161" s="4">
+        <v>1</v>
+      </c>
       <c r="J161" s="4"/>
     </row>
     <row r="162" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -5333,8 +5406,12 @@
       <c r="G162" s="4">
         <v>1</v>
       </c>
-      <c r="H162" s="4"/>
-      <c r="I162" s="4"/>
+      <c r="H162" s="4">
+        <v>1</v>
+      </c>
+      <c r="I162" s="4">
+        <v>1</v>
+      </c>
       <c r="J162" s="4"/>
     </row>
     <row r="163" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -5360,7 +5437,9 @@
         <v>1</v>
       </c>
       <c r="H163" s="4"/>
-      <c r="I163" s="4"/>
+      <c r="I163" s="4">
+        <v>1</v>
+      </c>
       <c r="J163" s="4"/>
     </row>
     <row r="164" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -5384,7 +5463,9 @@
       </c>
       <c r="G164" s="4"/>
       <c r="H164" s="4"/>
-      <c r="I164" s="4"/>
+      <c r="I164" s="4">
+        <v>1</v>
+      </c>
       <c r="J164" s="4"/>
     </row>
     <row r="165" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -5408,7 +5489,9 @@
       </c>
       <c r="G165" s="4"/>
       <c r="H165" s="4"/>
-      <c r="I165" s="4"/>
+      <c r="I165" s="4">
+        <v>1</v>
+      </c>
       <c r="J165" s="4"/>
     </row>
     <row r="166" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -5431,8 +5514,12 @@
       <c r="G166" s="4">
         <v>1</v>
       </c>
-      <c r="H166" s="4"/>
-      <c r="I166" s="4"/>
+      <c r="H166" s="4">
+        <v>1</v>
+      </c>
+      <c r="I166" s="4">
+        <v>1</v>
+      </c>
       <c r="J166" s="4"/>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
@@ -5458,7 +5545,9 @@
         <v>1</v>
       </c>
       <c r="H167" s="4"/>
-      <c r="I167" s="4"/>
+      <c r="I167" s="4">
+        <v>1</v>
+      </c>
       <c r="J167" s="4"/>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
@@ -5486,7 +5575,9 @@
       <c r="H168" s="4">
         <v>1</v>
       </c>
-      <c r="I168" s="4"/>
+      <c r="I168" s="4">
+        <v>1</v>
+      </c>
       <c r="J168" s="4"/>
     </row>
     <row r="169" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -5512,7 +5603,9 @@
       <c r="H169" s="4">
         <v>1</v>
       </c>
-      <c r="I169" s="4"/>
+      <c r="I169" s="4">
+        <v>1</v>
+      </c>
       <c r="J169" s="4"/>
     </row>
     <row r="170" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -5540,7 +5633,9 @@
       <c r="H170" s="4">
         <v>1</v>
       </c>
-      <c r="I170" s="4"/>
+      <c r="I170" s="4">
+        <v>1</v>
+      </c>
       <c r="J170" s="4"/>
     </row>
     <row r="171" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -5568,7 +5663,9 @@
       <c r="H171" s="4">
         <v>1</v>
       </c>
-      <c r="I171" s="4"/>
+      <c r="I171" s="4">
+        <v>1</v>
+      </c>
       <c r="J171" s="4"/>
     </row>
     <row r="172" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -5596,7 +5693,9 @@
       <c r="H172" s="4">
         <v>1</v>
       </c>
-      <c r="I172" s="4"/>
+      <c r="I172" s="4">
+        <v>1</v>
+      </c>
       <c r="J172" s="4"/>
     </row>
     <row r="173" spans="1:10" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
/ ‘Extended Campuses/Self Appraisals/2015/Raw Data from SQL Query for 2015.xlsx’ / ‘Extended Campuses/Self Appraisals/2015/Talbert Tso Performance Appraisal for Applications Systems Analyst.doc’
</commit_message>
<xml_diff>
--- a/Extended Campuses/Self Appraisals/2015/Raw Data from SQL Query for 2015.xlsx
+++ b/Extended Campuses/Self Appraisals/2015/Raw Data from SQL Query for 2015.xlsx
@@ -1407,7 +1407,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1418,6 +1418,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1437,7 +1444,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1448,6 +1455,11 @@
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -1491,13 +1503,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1509,19 +1522,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1802,8 +1818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J438"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2485,7 +2501,7 @@
       <c r="E31" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="13">
         <v>1</v>
       </c>
       <c r="I31" s="7">
@@ -2508,7 +2524,7 @@
       <c r="E32" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="13">
         <v>1</v>
       </c>
       <c r="I32" s="7">
@@ -2531,7 +2547,7 @@
       <c r="E33" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F33" s="7"/>
+      <c r="F33" s="13"/>
       <c r="I33" s="7"/>
     </row>
     <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2611,7 +2627,7 @@
       <c r="E37" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F37" s="4"/>
+      <c r="F37" s="14"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
@@ -2633,7 +2649,7 @@
       <c r="E38" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F38" s="14">
         <v>1</v>
       </c>
       <c r="G38" s="4"/>
@@ -2657,7 +2673,7 @@
       <c r="E39" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F39" s="4"/>
+      <c r="F39" s="14"/>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
@@ -2679,7 +2695,7 @@
       <c r="E40" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F40" s="4"/>
+      <c r="F40" s="14"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
@@ -2779,7 +2795,7 @@
       <c r="E45" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F45" s="13">
         <v>1</v>
       </c>
     </row>
@@ -2799,6 +2815,7 @@
       <c r="E46" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="F46" s="13"/>
     </row>
     <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
@@ -2816,7 +2833,7 @@
       <c r="E47" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F47" s="4">
+      <c r="F47" s="13">
         <v>1</v>
       </c>
       <c r="G47" s="4"/>
@@ -2840,7 +2857,7 @@
       <c r="E48" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F48" s="4"/>
+      <c r="F48" s="13"/>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
@@ -2862,7 +2879,7 @@
       <c r="E49" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F49" s="4"/>
+      <c r="F49" s="13"/>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
@@ -2884,7 +2901,7 @@
       <c r="E50" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F50" s="4">
+      <c r="F50" s="13">
         <v>1</v>
       </c>
       <c r="G50" s="4"/>
@@ -2908,7 +2925,7 @@
       <c r="E51" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F51" s="4"/>
+      <c r="F51" s="13"/>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
@@ -2930,7 +2947,7 @@
       <c r="E52" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F52" s="4"/>
+      <c r="F52" s="13"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
@@ -2952,7 +2969,7 @@
       <c r="E53" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F53" s="1">
+      <c r="F53" s="13">
         <v>1</v>
       </c>
     </row>
@@ -2972,6 +2989,7 @@
       <c r="E54" s="3" t="s">
         <v>67</v>
       </c>
+      <c r="F54" s="13"/>
     </row>
     <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
@@ -2983,13 +3001,13 @@
       <c r="C55" s="4">
         <v>4</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="11" t="s">
         <v>68</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F55" s="4">
+      <c r="F55" s="13">
         <v>1</v>
       </c>
       <c r="G55" s="4"/>
@@ -3015,7 +3033,7 @@
       <c r="E56" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F56" s="4">
+      <c r="F56" s="13">
         <v>1</v>
       </c>
       <c r="G56" s="4"/>
@@ -3045,7 +3063,7 @@
       <c r="E57" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F57" s="4">
+      <c r="F57" s="13">
         <v>1</v>
       </c>
       <c r="G57" s="4"/>
@@ -3073,7 +3091,7 @@
       <c r="E58" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F58" s="4">
+      <c r="F58" s="13">
         <v>1</v>
       </c>
       <c r="G58" s="4"/>
@@ -3101,7 +3119,7 @@
       <c r="E59" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F59" s="4">
+      <c r="F59" s="13">
         <v>1</v>
       </c>
       <c r="G59" s="4"/>
@@ -3129,7 +3147,7 @@
       <c r="E60" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F60" s="4"/>
+      <c r="F60" s="13"/>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
@@ -3151,7 +3169,7 @@
       <c r="E61" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F61" s="1">
+      <c r="F61" s="13">
         <v>1</v>
       </c>
       <c r="J61" s="1">
@@ -3174,7 +3192,7 @@
       <c r="E62" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F62" s="1">
+      <c r="F62" s="13">
         <v>1</v>
       </c>
       <c r="H62" s="1">
@@ -3197,7 +3215,7 @@
       <c r="E63" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F63" s="1">
+      <c r="F63" s="13">
         <v>1</v>
       </c>
       <c r="H63" s="1">
@@ -3220,6 +3238,7 @@
       <c r="E64" s="3" t="s">
         <v>79</v>
       </c>
+      <c r="F64" s="13"/>
     </row>
     <row r="65" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
@@ -3237,6 +3256,7 @@
       <c r="E65" s="3" t="s">
         <v>80</v>
       </c>
+      <c r="F65" s="13"/>
     </row>
     <row r="66" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
@@ -3254,6 +3274,7 @@
       <c r="E66" s="3" t="s">
         <v>81</v>
       </c>
+      <c r="F66" s="13"/>
     </row>
     <row r="67" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="4">

</xml_diff>